<commit_message>
Update resources and DataFrames
</commit_message>
<xml_diff>
--- a/Resources/LivingWagesWorkingPoor.xlsx
+++ b/Resources/LivingWagesWorkingPoor.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Denise\Desktop\LivingWagesWorkingPoor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Denise\Desktop\LivingWagesRepo\LivingWages-WorkingPoor\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9AF1B666-304D-4355-9EC4-8DEE8AA491DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F5F0A0-F398-457D-952E-2E62CC6D71C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="12465" windowHeight="6915" xr2:uid="{127C7B8F-5309-466E-B311-582D75BF90E4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{127C7B8F-5309-466E-B311-582D75BF90E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -633,13 +633,13 @@
   <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="58.28515625" customWidth="1"/>
     <col min="2" max="2" width="56.28515625" customWidth="1"/>
     <col min="3" max="3" width="78.140625" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
We created TANF DF for 2019
</commit_message>
<xml_diff>
--- a/Resources/LivingWagesWorkingPoor.xlsx
+++ b/Resources/LivingWagesWorkingPoor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Pictures\Head Shots\LivingWagesWorkingPoor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Denise\Desktop\LivingWagesRepo\LivingWages-WorkingPoor\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901AE953-D442-4FB0-9112-0C0CD7193AE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A66A9B0-3EE6-49D8-90A3-9EDF1CCB42F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="15945" windowHeight="10155" activeTab="1" xr2:uid="{127C7B8F-5309-466E-B311-582D75BF90E4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{127C7B8F-5309-466E-B311-582D75BF90E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Data sites" sheetId="1" r:id="rId1"/>
@@ -2379,7 +2379,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>